<commit_message>
feat: integração e verificador de cartões
</commit_message>
<xml_diff>
--- a/tabela_nomes.xlsx
+++ b/tabela_nomes.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26306"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD2BB309-9618-4852-9818-5F1A50D16FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\repos\ExcelToTrello\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{19C5BE0D-F59E-4FCA-B1D1-21791A7B9C83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,24 +16,11 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Nome</t>
   </si>
@@ -144,9 +136,6 @@
     <t>Guilherme Alves</t>
   </si>
   <si>
-    <t>369.852.147-00</t>
-  </si>
-  <si>
     <t>Pedro Leite</t>
   </si>
   <si>
@@ -175,6 +164,9 @@
   </si>
   <si>
     <t>Gabrihel Bieguelman</t>
+  </si>
+  <si>
+    <t>987.654.321-01</t>
   </si>
 </sst>
 </file>
@@ -265,7 +257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -561,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -725,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -734,18 +726,18 @@
         <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>20</v>
@@ -754,18 +746,18 @@
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>25</v>
@@ -774,18 +766,18 @@
         <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>30</v>
@@ -794,7 +786,27 @@
         <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>48</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>